<commit_message>
XLSX import : ignore unknown columsn
</commit_message>
<xml_diff>
--- a/misc/event-import.xlsx
+++ b/misc/event-import.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aurels/Dev/sitcom/sitcom/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D8C7D7-37FA-7845-BDB4-C4A46AA5B633}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D99192-4DC1-6747-B66F-D266318018F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16400" xr2:uid="{C6E3FA61-672D-344C-A58C-7C9DE9A2D89E}"/>
   </bookViews>
@@ -64,9 +64,6 @@
     <t>Lieu</t>
   </si>
   <si>
-    <t>Site web (URL)</t>
-  </si>
-  <si>
     <t>Mundaneum</t>
   </si>
   <si>
@@ -86,6 +83,9 @@
   </si>
   <si>
     <t>Salle de conférence b1</t>
+  </si>
+  <si>
+    <t>Site web</t>
   </si>
 </sst>
 </file>
@@ -446,7 +446,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -471,38 +471,38 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
       </c>
       <c r="C2" s="2">
         <v>42933</v>
       </c>
       <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2">
         <v>43093</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>